<commit_message>
[WIP] remove references to earlier project with tutorials
</commit_message>
<xml_diff>
--- a/node-express-server/salesTemplate.xlsx
+++ b/node-express-server/salesTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\angular\boilerPlate\EcoSochSalesForm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\angular\boilerPlate\es-excel-export\node-express-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4551B8B9-05BF-451A-A576-6ACB909909FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE0E4C8-7585-47F3-8055-6795F40B2F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1827" yWindow="1300" windowWidth="12800" windowHeight="7180" xr2:uid="{B5F2AF2D-B049-4A1E-B44B-C5C78171A5DE}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="17253" windowHeight="10133" xr2:uid="{B5F2AF2D-B049-4A1E-B44B-C5C78171A5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,13 @@
     <t>Sanctioned Load (in kW)</t>
   </si>
   <si>
-    <t>Phase at Premises</t>
-  </si>
-  <si>
     <t>Single Phase</t>
   </si>
   <si>
     <t xml:space="preserve">power </t>
+  </si>
+  <si>
+    <t>Phase at Premises?</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -409,15 +409,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <f>B1*1000</f>

</xml_diff>